<commit_message>
update csv and excel again
</commit_message>
<xml_diff>
--- a/Artists/Lyrics_Analysis.xlsx
+++ b/Artists/Lyrics_Analysis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B95"/>
+  <dimension ref="A1:B116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -604,403 +604,403 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Chorus 1</t>
+          <t>Bridge 1</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>'Cause I'm the only one who understands</t>
+          <t>Like I'm the only one that's in command</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Chorus 2</t>
+          <t>Bridge 2</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Want you to make me feel like I'm the only girl in the world</t>
+          <t>Only one</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Chorus 3</t>
+          <t>Bridge 3</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Like I'm the only one that you'll ever love</t>
+          <t>Only one</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Chorus 4</t>
+          <t>Bridge 4</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Like I'm the only one who knows your heart</t>
+          <t>Take me for a ride, ride</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Chorus 5</t>
+          <t>Bridge 5</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Want you to make me feel like I'm the only girl in the world</t>
+          <t>Oh, baby, take me high, high</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Chorus 6</t>
+          <t>Bridge 6</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Like I'm the only one that you'll ever love</t>
+          <t>Let me make you rise, rise</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Chorus 7</t>
+          <t>Bridge 7</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Like I'm the only one who knows your heart</t>
+          <t>Take me for a ride, ride</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Chorus 8</t>
+          <t>Bridge 8</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>'Cause I'm the only one who understands</t>
+          <t>Oh, baby, take me high, high</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Chorus 9</t>
+          <t>Bridge 9</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Like I'm the only one who knows your heart</t>
+          <t>Let me make you rise, rise</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Chorus 10</t>
+          <t>Bridge 10</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Want you to make me feel like I'm the only girl in the world</t>
+          <t>Oh, baby, take me high, high</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Chorus 11</t>
+          <t>Bridge 11</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Like I'm the only one that you'll ever love</t>
+          <t>Let me make you rise, rise</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Chorus 12</t>
+          <t>Bridge 12</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Like I'm the only one who knows your heart</t>
+          <t>Let me make you rise, rise</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Chorus 13</t>
+          <t>Bridge 13</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Only girl in the world</t>
+          <t>Take me for a ride, ride</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Chorus 14</t>
+          <t>Bridge 14</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>'Cause I'm the only one who understands</t>
+          <t>Oh, baby, take me high, high</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Chorus 15</t>
+          <t>Bridge 15</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Only girl in the world</t>
+          <t>Let me make you rise, rise</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Chorus 16</t>
+          <t>Bridge 16</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Only girl in the world</t>
+          <t>Oh, baby, take me high, high</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Chorus 17</t>
+          <t>Bridge 17</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Want you to make me feel like I'm the only girl in the world</t>
+          <t>Let me make you rise, rise</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Chorus 18</t>
+          <t>Bridge 18</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Like I'm the only one that you'll ever love</t>
+          <t>Let me make you rise, rise</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Chorus 19</t>
+          <t>Bridge 19</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Like I'm the only one who knows your heart</t>
+          <t>Like I'm the only one that's in command</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Chorus 20</t>
+          <t>Bridge 20</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>'Cause I'm the only one who understands</t>
+          <t>Girl in the world</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Chorus 21</t>
+          <t>Bridge 21</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Like I'm the only one who knows your heart</t>
+          <t>Girl in the world</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Chorus 22</t>
+          <t>Chorus 1</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Want you to make me feel like I'm the only girl in the world</t>
+          <t>'Cause I'm the only one who understands</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Chorus 23</t>
+          <t>Chorus 2</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Like I'm the only one that you'll ever love</t>
+          <t>Want you to make me feel like I'm the only girl in the world</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Chorus 24</t>
+          <t>Chorus 3</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Like I'm the only one who knows your heart</t>
+          <t>Like I'm the only one that you'll ever love</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Chorus 25</t>
+          <t>Chorus 4</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Only girl in the world</t>
+          <t>Like I'm the only one who knows your heart</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Chorus 26</t>
+          <t>Chorus 5</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>'Cause I'm the only one who understands</t>
+          <t>Want you to make me feel like I'm the only girl in the world</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Chorus 27</t>
+          <t>Chorus 6</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Only girl in the world</t>
+          <t>Like I'm the only one that you'll ever love</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Chorus 28</t>
+          <t>Chorus 7</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Only girl in the world</t>
+          <t>Like I'm the only one who knows your heart</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Chorus 29</t>
+          <t>Chorus 8</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Want you to make me feel like I'm the only girl in the world</t>
+          <t>'Cause I'm the only one who understands</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Chorus 30</t>
+          <t>Chorus 9</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Like I'm the only one that you'll ever love</t>
+          <t>Like I'm the only one who knows your heart</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Chorus 31</t>
+          <t>Chorus 10</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Like I'm the only one who knows your heart</t>
+          <t>Want you to make me feel like I'm the only girl in the world</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Chorus 32</t>
+          <t>Chorus 11</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Only girl in the world</t>
+          <t>Like I'm the only one that you'll ever love</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Chorus 33</t>
+          <t>Chorus 12</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>'Cause I'm the only one who understands</t>
+          <t>Like I'm the only one who knows your heart</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Chorus 34</t>
+          <t>Chorus 13</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1012,103 +1012,103 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Chorus 35</t>
+          <t>Chorus 14</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Only girl in the world</t>
+          <t>'Cause I'm the only one who understands</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Chorus 36</t>
+          <t>Chorus 15</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Want you to make me feel like I'm the only girl in the world</t>
+          <t>Only girl in the world</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Chorus 37</t>
+          <t>Chorus 16</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Like I'm the only one that you'll ever love</t>
+          <t>Only girl in the world</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Chorus 38</t>
+          <t>Chorus 17</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Like I'm the only one who knows your heart</t>
+          <t>Want you to make me feel like I'm the only girl in the world</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Chorus 39</t>
+          <t>Chorus 18</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Only girl in the world</t>
+          <t>Like I'm the only one that you'll ever love</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Chorus 40</t>
+          <t>Chorus 19</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>'Cause I'm the only one who understands</t>
+          <t>Like I'm the only one who knows your heart</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Chorus 41</t>
+          <t>Chorus 20</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Only girl in the world</t>
+          <t>'Cause I'm the only one who understands</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Chorus 42</t>
+          <t>Chorus 21</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Only girl in the world</t>
+          <t>Like I'm the only one who knows your heart</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Chorus 43</t>
+          <t>Chorus 22</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1120,7 +1120,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Chorus 44</t>
+          <t>Chorus 23</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1132,7 +1132,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Chorus 45</t>
+          <t>Chorus 24</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1144,7 +1144,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Chorus 46</t>
+          <t>Chorus 25</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1156,7 +1156,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Chorus 47</t>
+          <t>Chorus 26</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1168,7 +1168,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Chorus 48</t>
+          <t>Chorus 27</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1180,7 +1180,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Chorus 49</t>
+          <t>Chorus 28</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1192,7 +1192,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Chorus 50</t>
+          <t>Chorus 29</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1204,7 +1204,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Chorus 51</t>
+          <t>Chorus 30</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1216,7 +1216,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Chorus 52</t>
+          <t>Chorus 31</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1228,7 +1228,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Chorus 53</t>
+          <t>Chorus 32</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1240,7 +1240,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Chorus 54</t>
+          <t>Chorus 33</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1252,7 +1252,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Chorus 55</t>
+          <t>Chorus 34</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1264,7 +1264,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Chorus 56</t>
+          <t>Chorus 35</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -1276,7 +1276,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Chorus 57</t>
+          <t>Chorus 36</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1288,7 +1288,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Chorus 58</t>
+          <t>Chorus 37</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -1300,7 +1300,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Chorus 59</t>
+          <t>Chorus 38</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -1312,7 +1312,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Chorus 60</t>
+          <t>Chorus 39</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -1324,7 +1324,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Chorus 61</t>
+          <t>Chorus 40</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -1336,7 +1336,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Chorus 62</t>
+          <t>Chorus 41</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1348,7 +1348,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Chorus 63</t>
+          <t>Chorus 42</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1360,7 +1360,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Chorus 64</t>
+          <t>Chorus 43</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1372,7 +1372,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Chorus 65</t>
+          <t>Chorus 44</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -1384,7 +1384,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Chorus 66</t>
+          <t>Chorus 45</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -1396,7 +1396,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Chorus 67</t>
+          <t>Chorus 46</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -1408,7 +1408,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Chorus 68</t>
+          <t>Chorus 47</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -1420,7 +1420,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Chorus 69</t>
+          <t>Chorus 48</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -1432,7 +1432,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Chorus 70</t>
+          <t>Chorus 49</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -1444,7 +1444,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Chorus 71</t>
+          <t>Chorus 50</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -1456,7 +1456,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Chorus 72</t>
+          <t>Chorus 51</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -1468,7 +1468,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Chorus 73</t>
+          <t>Chorus 52</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1480,7 +1480,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Chorus 74</t>
+          <t>Chorus 53</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -1492,7 +1492,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Chorus 75</t>
+          <t>Chorus 54</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -1504,7 +1504,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Chorus 76</t>
+          <t>Chorus 55</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -1516,7 +1516,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Chorus 77</t>
+          <t>Chorus 56</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -1528,46 +1528,298 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Chorus 78</t>
+          <t>Chorus 57</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>'Cause I'm the only one who understands</t>
+          <t>Want you to make me feel like I'm the only girl in the world</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Chorus 79</t>
+          <t>Chorus 58</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Only girl in the world</t>
+          <t>Like I'm the only one that you'll ever love</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Chorus 80</t>
+          <t>Chorus 59</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Only girl in the world</t>
+          <t>Like I'm the only one who knows your heart</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
+          <t>Chorus 60</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Only girl in the world</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Chorus 61</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>'Cause I'm the only one who understands</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Chorus 62</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Only girl in the world</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Chorus 63</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Only girl in the world</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Chorus 64</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Want you to make me feel like I'm the only girl in the world</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Chorus 65</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Like I'm the only one that you'll ever love</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Chorus 66</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Like I'm the only one who knows your heart</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Chorus 67</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Only girl in the world</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Chorus 68</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>'Cause I'm the only one who understands</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Chorus 69</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Only girl in the world</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Chorus 70</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Only girl in the world</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Chorus 71</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Want you to make me feel like I'm the only girl in the world</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Chorus 72</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Like I'm the only one that you'll ever love</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Chorus 73</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Like I'm the only one who knows your heart</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Chorus 74</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Only girl in the world</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Chorus 75</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>'Cause I'm the only one who understands</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Chorus 76</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Only girl in the world</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Chorus 77</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Only girl in the world</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Chorus 78</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>'Cause I'm the only one who understands</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Chorus 79</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Only girl in the world</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Chorus 80</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Only girl in the world</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
           <t>Chorus 81</t>
         </is>
       </c>
-      <c r="B95" t="inlineStr">
+      <c r="B116" t="inlineStr">
         <is>
           <t>Only girl in the world</t>
         </is>

</xml_diff>